<commit_message>
Got multicolumn (but not multirow) working
</commit_message>
<xml_diff>
--- a/Example/simple_table.xlsx
+++ b/Example/simple_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="0" windowWidth="27840" windowHeight="13020"/>
+    <workbookView xWindow="2880" yWindow="0" windowWidth="27840" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>row label 1</t>
   </si>
@@ -48,14 +48,63 @@
   </si>
   <si>
     <t>column label 3</t>
+  </si>
+  <si>
+    <t>merged cell here</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,10 +152,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,19 +453,23 @@
     <col min="2" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -424,9 +482,15 @@
       <c r="D2">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -438,8 +502,14 @@
       <c r="D3">
         <v>4.5</v>
       </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -452,8 +522,14 @@
       <c r="D4" s="2">
         <v>345.34500000000003</v>
       </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -466,8 +542,14 @@
       <c r="D5">
         <v>999</v>
       </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -480,8 +562,18 @@
       <c r="D6" s="2">
         <v>7</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>